<commit_message>
Updated tools sheet and map.
</commit_message>
<xml_diff>
--- a/remnux-tools-sheet.xlsx
+++ b/remnux-tools-sheet.xlsx
@@ -15,14 +15,14 @@
     <sheet name="REMnux Tools" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REMnux Tools'!$A$1:$F$166</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REMnux Tools'!$A$1:$F$168</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="772">
   <si>
     <t>AnalyzePDF</t>
   </si>
@@ -2322,6 +2322,33 @@
   </si>
   <si>
     <t>https://code.google.com/p/origami-pdf/</t>
+  </si>
+  <si>
+    <t>PyInstaller Extractor</t>
+  </si>
+  <si>
+    <t>pyinstxtractor.py</t>
+  </si>
+  <si>
+    <t>Extract contents of a Windows executable file generated using PyInstaller</t>
+  </si>
+  <si>
+    <t>https://sourceforge.net/projects/pyinstallerextractor/</t>
+  </si>
+  <si>
+    <t>Decompyle++</t>
+  </si>
+  <si>
+    <t>pycdas, pycdc</t>
+  </si>
+  <si>
+    <t>Python bytecode disassembler and decompiler</t>
+  </si>
+  <si>
+    <t>remnux-pycdc (APT)</t>
+  </si>
+  <si>
+    <t>https://github.com/zrax/pycdc</t>
   </si>
 </sst>
 </file>
@@ -2691,11 +2718,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F166"/>
+  <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5544,22 +5571,22 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
-        <v>58</v>
+        <v>632</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>57</v>
+        <v>767</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>669</v>
+        <v>768</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E144" s="6" t="s">
-        <v>667</v>
+        <v>769</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>770</v>
       </c>
       <c r="F144" s="9" t="s">
-        <v>60</v>
+        <v>771</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
@@ -5567,59 +5594,59 @@
         <v>58</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>383</v>
+        <v>57</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>384</v>
+        <v>669</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>603</v>
+        <v>59</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>602</v>
+        <v>667</v>
       </c>
       <c r="F145" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>90</v>
+        <v>383</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>671</v>
+        <v>384</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>670</v>
+        <v>603</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>672</v>
+        <v>602</v>
       </c>
       <c r="F146" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>138</v>
+        <v>671</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>139</v>
+        <v>670</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>542</v>
+        <v>672</v>
       </c>
       <c r="F147" s="9" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
@@ -5627,39 +5654,39 @@
         <v>58</v>
       </c>
       <c r="B148" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="F148" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B149" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C148" s="5" t="s">
+      <c r="C149" s="5" t="s">
         <v>648</v>
       </c>
-      <c r="D148" s="5" t="s">
+      <c r="D149" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E148" s="6" t="s">
+      <c r="E149" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="F148" s="9" t="s">
+      <c r="F149" s="9" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A149" s="5" t="s">
-        <v>755</v>
-      </c>
-      <c r="B149" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D149" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E149" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="F149" s="9" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -5667,19 +5694,19 @@
         <v>755</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>309</v>
+        <v>244</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>310</v>
+        <v>244</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>245</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>604</v>
+        <v>525</v>
       </c>
       <c r="F150" s="9" t="s">
-        <v>311</v>
+        <v>246</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -5687,79 +5714,79 @@
         <v>755</v>
       </c>
       <c r="B151" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D151" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E151" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="F151" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A152" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="B152" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C151" s="5" t="s">
+      <c r="C152" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="D151" s="5" t="s">
+      <c r="D152" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E151" s="6" t="s">
+      <c r="E152" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="F151" s="9" t="s">
+      <c r="F152" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A152" s="5" t="s">
+    <row r="153" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A153" s="5" t="s">
         <v>756</v>
       </c>
-      <c r="B152" s="5" t="s">
+      <c r="B153" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C152" s="5" t="s">
+      <c r="C153" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D152" s="5" t="s">
+      <c r="D153" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E152" s="6" t="s">
+      <c r="E153" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="F152" s="9" t="s">
+      <c r="F153" s="9" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" s="6" t="s">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="B153" s="6" t="s">
+      <c r="B154" s="6" t="s">
         <v>565</v>
       </c>
-      <c r="C153" s="6" t="s">
+      <c r="C154" s="6" t="s">
         <v>565</v>
       </c>
-      <c r="D153" s="6" t="s">
+      <c r="D154" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="E153" s="6" t="s">
+      <c r="E154" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="F153" s="9" t="s">
+      <c r="F154" s="9" t="s">
         <v>566</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="B154" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C154" s="5" t="s">
-        <v>610</v>
-      </c>
-      <c r="D154" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="E154" s="6" t="s">
-        <v>609</v>
-      </c>
-      <c r="F154" s="9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
@@ -5767,19 +5794,19 @@
         <v>756</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>269</v>
+        <v>79</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>269</v>
+        <v>610</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>270</v>
+        <v>757</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>451</v>
+        <v>609</v>
       </c>
       <c r="F155" s="9" t="s">
-        <v>271</v>
+        <v>80</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -5787,19 +5814,19 @@
         <v>756</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>400</v>
+        <v>269</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>401</v>
+        <v>269</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>402</v>
+        <v>270</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>649</v>
+        <v>451</v>
       </c>
       <c r="F156" s="9" t="s">
-        <v>403</v>
+        <v>271</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -5807,198 +5834,238 @@
         <v>756</v>
       </c>
       <c r="B157" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="D157" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E157" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="F157" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="B158" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C157" s="5" t="s">
+      <c r="C158" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D157" s="5" t="s">
+      <c r="D158" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E157" s="6" t="s">
+      <c r="E158" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="F157" s="9" t="s">
+      <c r="F158" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A158" s="5" t="s">
-        <v>758</v>
-      </c>
-      <c r="B158" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C158" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="D158" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E158" s="6" t="s">
-        <v>664</v>
-      </c>
-      <c r="F158" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
         <v>758</v>
       </c>
       <c r="B159" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="D159" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E159" s="6" t="s">
+        <v>664</v>
+      </c>
+      <c r="F159" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B160" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="C159" s="5" t="s">
+      <c r="C160" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="D159" s="5" t="s">
+      <c r="D160" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E159" s="5" t="s">
+      <c r="E160" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="F159" s="9" t="s">
+      <c r="F160" s="9" t="s">
         <v>662</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A160" s="5" t="s">
-        <v>759</v>
-      </c>
-      <c r="B160" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C160" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D160" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E160" s="6" t="s">
-        <v>528</v>
-      </c>
-      <c r="F160" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="E161" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="F161" s="9" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A162" s="5" t="s">
         <v>759</v>
       </c>
-      <c r="B161" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D161" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E161" s="6" t="s">
-        <v>531</v>
-      </c>
-      <c r="F161" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A162" s="5" t="s">
-        <v>760</v>
-      </c>
       <c r="B162" s="5" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>505</v>
+        <v>528</v>
       </c>
       <c r="F162" s="9" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>169</v>
+        <v>272</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>170</v>
+        <v>273</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>171</v>
+        <v>274</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>684</v>
+        <v>531</v>
       </c>
       <c r="F163" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>175</v>
+        <v>87</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>176</v>
+        <v>88</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>666</v>
+        <v>505</v>
       </c>
       <c r="F164" s="9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
         <v>761</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>254</v>
+        <v>169</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>255</v>
+        <v>170</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>256</v>
+        <v>171</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>451</v>
+        <v>684</v>
       </c>
       <c r="F165" s="9" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>761</v>
       </c>
       <c r="B166" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E166" s="6" t="s">
+        <v>666</v>
+      </c>
+      <c r="F166" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C167" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D167" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E167" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="F167" s="9" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A168" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="B168" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="C166" s="5" t="s">
+      <c r="C168" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="D166" s="5" t="s">
+      <c r="D168" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="E166" s="6" t="s">
+      <c r="E168" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="F166" s="9" t="s">
+      <c r="F168" s="9" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6142,34 +6209,36 @@
     <hyperlink ref="F141" r:id="rId132"/>
     <hyperlink ref="F142" r:id="rId133"/>
     <hyperlink ref="F143" r:id="rId134"/>
-    <hyperlink ref="F144" r:id="rId135"/>
-    <hyperlink ref="F145" r:id="rId136"/>
-    <hyperlink ref="F146" r:id="rId137"/>
-    <hyperlink ref="F147" r:id="rId138"/>
-    <hyperlink ref="F148" r:id="rId139"/>
-    <hyperlink ref="F149" r:id="rId140"/>
-    <hyperlink ref="F150" r:id="rId141"/>
-    <hyperlink ref="F151" r:id="rId142"/>
-    <hyperlink ref="F152" r:id="rId143"/>
-    <hyperlink ref="F153" r:id="rId144"/>
-    <hyperlink ref="F154" r:id="rId145"/>
-    <hyperlink ref="F155" r:id="rId146"/>
-    <hyperlink ref="F156" r:id="rId147"/>
-    <hyperlink ref="F157" r:id="rId148"/>
-    <hyperlink ref="F158" r:id="rId149"/>
-    <hyperlink ref="F159" r:id="rId150"/>
-    <hyperlink ref="F160" r:id="rId151"/>
-    <hyperlink ref="F161" r:id="rId152"/>
-    <hyperlink ref="F162" r:id="rId153"/>
-    <hyperlink ref="F163" r:id="rId154"/>
-    <hyperlink ref="F164" r:id="rId155"/>
-    <hyperlink ref="F165" r:id="rId156"/>
-    <hyperlink ref="F166" r:id="rId157"/>
+    <hyperlink ref="F145" r:id="rId135"/>
+    <hyperlink ref="F146" r:id="rId136"/>
+    <hyperlink ref="F147" r:id="rId137"/>
+    <hyperlink ref="F148" r:id="rId138"/>
+    <hyperlink ref="F149" r:id="rId139"/>
+    <hyperlink ref="F150" r:id="rId140"/>
+    <hyperlink ref="F151" r:id="rId141"/>
+    <hyperlink ref="F152" r:id="rId142"/>
+    <hyperlink ref="F153" r:id="rId143"/>
+    <hyperlink ref="F154" r:id="rId144"/>
+    <hyperlink ref="F155" r:id="rId145"/>
+    <hyperlink ref="F156" r:id="rId146"/>
+    <hyperlink ref="F157" r:id="rId147"/>
+    <hyperlink ref="F158" r:id="rId148"/>
+    <hyperlink ref="F159" r:id="rId149"/>
+    <hyperlink ref="F160" r:id="rId150"/>
+    <hyperlink ref="F162" r:id="rId151"/>
+    <hyperlink ref="F163" r:id="rId152"/>
+    <hyperlink ref="F164" r:id="rId153"/>
+    <hyperlink ref="F165" r:id="rId154"/>
+    <hyperlink ref="F166" r:id="rId155"/>
+    <hyperlink ref="F167" r:id="rId156"/>
+    <hyperlink ref="F168" r:id="rId157"/>
+    <hyperlink ref="F161" r:id="rId158"/>
+    <hyperlink ref="F144" r:id="rId159"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId158"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId160"/>
   <webPublishItems count="1">
-    <webPublishItem id="28559" divId="remnux-tools_28559" sourceType="sheet" destinationFile="C:\Users\Lenny\Documents\SANS Institute\REMnux\v6\remnux-tools.html" title="REMnux Tools"/>
+    <webPublishItem id="28559" divId="remnux-tools_28559" sourceType="sheet" destinationFile="C:\Users\Lenny\Documents\SANS Institute\REMnux\v6\remnux-tools-sheet.html" title="REMnux Tools"/>
   </webPublishItems>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated tools map and sheet.
</commit_message>
<xml_diff>
--- a/remnux-tools-sheet.xlsx
+++ b/remnux-tools-sheet.xlsx
@@ -15,14 +15,14 @@
     <sheet name="REMnux Tools" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REMnux Tools'!$A$1:$F$168</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'REMnux Tools'!$A$1:$F$169</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="777">
   <si>
     <t>AnalyzePDF</t>
   </si>
@@ -2349,6 +2349,21 @@
   </si>
   <si>
     <t>https://github.com/zrax/pycdc</t>
+  </si>
+  <si>
+    <t>VirusTotalApi</t>
+  </si>
+  <si>
+    <t>vt</t>
+  </si>
+  <si>
+    <t>Retrieve data from VirusTotal</t>
+  </si>
+  <si>
+    <t>remnux-virustotalapi (APT)</t>
+  </si>
+  <si>
+    <t>https://github.com/doomedraven/VirusTotalApi</t>
   </si>
 </sst>
 </file>
@@ -2718,11 +2733,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F168"/>
+  <dimension ref="A1:F169"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4105,63 +4120,61 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>354</v>
-      </c>
+      <c r="A70" s="6"/>
       <c r="B70" s="5" t="s">
-        <v>352</v>
+        <v>772</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>353</v>
+        <v>773</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>355</v>
+        <v>774</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>455</v>
+        <v>775</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>356</v>
+        <v>776</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>573</v>
+        <v>354</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>497</v>
+        <v>352</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>500</v>
+        <v>353</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>572</v>
+        <v>355</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>498</v>
+        <v>356</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>354</v>
+        <v>573</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>364</v>
+        <v>497</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>365</v>
+        <v>500</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>366</v>
+        <v>572</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>367</v>
+        <v>498</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -4169,76 +4182,79 @@
         <v>354</v>
       </c>
       <c r="B73" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>587</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D74" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="E74" s="6" t="s">
         <v>582</v>
       </c>
-      <c r="F73" s="9" t="s">
+      <c r="F74" s="9" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B75" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C75" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D75" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="E74" s="6" t="s">
+      <c r="E75" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="F74" s="9" t="s">
+      <c r="F75" s="9" t="s">
         <v>539</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>550</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>495</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>128</v>
+        <v>354</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>159</v>
+        <v>434</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>160</v>
+        <v>435</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>457</v>
+        <v>550</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -4246,136 +4262,133 @@
         <v>128</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>204</v>
+        <v>159</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="E77" s="5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="F78" s="9" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B79" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C79" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="D79" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="E79" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="F78" s="9" t="s">
+      <c r="F79" s="9" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>425</v>
+        <v>280</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>699</v>
+        <v>281</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B81" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>701</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D82" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="E82" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="F81" s="9" t="s">
+      <c r="F82" s="9" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>749</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>460</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>35</v>
+        <v>346</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>36</v>
+        <v>749</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>38</v>
+        <v>347</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>39</v>
+        <v>750</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -4383,19 +4396,19 @@
         <v>37</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>210</v>
+        <v>35</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>211</v>
+        <v>36</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>212</v>
+        <v>38</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>496</v>
+        <v>461</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>213</v>
+        <v>39</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -4403,19 +4416,19 @@
         <v>37</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>76</v>
+        <v>210</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>76</v>
+        <v>211</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>77</v>
+        <v>212</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>451</v>
+        <v>496</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>78</v>
+        <v>213</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -4423,99 +4436,99 @@
         <v>37</v>
       </c>
       <c r="B86" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D87" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="E87" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="F86" s="9" t="s">
+      <c r="F87" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A87" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>165</v>
+        <v>11</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>167</v>
+        <v>13</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>28</v>
+        <v>166</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>29</v>
+        <v>167</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>451</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>240</v>
+        <v>27</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>241</v>
+        <v>28</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>242</v>
+        <v>29</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>451</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>243</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -4523,19 +4536,19 @@
         <v>12</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>133</v>
+        <v>240</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>134</v>
+        <v>241</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>135</v>
+        <v>242</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>451</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>136</v>
+        <v>243</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -4543,99 +4556,99 @@
         <v>12</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>330</v>
+        <v>133</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>331</v>
+        <v>134</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>332</v>
+        <v>135</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>451</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>427</v>
+        <v>330</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>428</v>
+        <v>331</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>429</v>
+        <v>332</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>151</v>
+        <v>427</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>152</v>
+        <v>428</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>153</v>
+        <v>429</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>452</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B95" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A96" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C96" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D96" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="E95" s="6" t="s">
+      <c r="E96" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="F95" s="9" t="s">
+      <c r="F96" s="9" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="E96" s="6" t="s">
-        <v>649</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -4643,99 +4656,99 @@
         <v>109</v>
       </c>
       <c r="B97" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C98" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D98" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E97" s="6" t="s">
+      <c r="E98" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="F97" s="9" t="s">
+      <c r="F98" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>607</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>206</v>
+        <v>607</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>207</v>
+        <v>23</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>208</v>
+        <v>25</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>480</v>
+        <v>608</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>209</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="5" t="s">
         <v>752</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B101" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C101" s="5" t="s">
         <v>612</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D101" s="5" t="s">
         <v>613</v>
       </c>
-      <c r="E100" s="5" t="s">
+      <c r="E101" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="F100" s="9" t="s">
+      <c r="F101" s="9" t="s">
         <v>614</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A101" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>481</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -4743,39 +4756,39 @@
         <v>114</v>
       </c>
       <c r="B102" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C103" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D103" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E102" s="6" t="s">
+      <c r="E103" s="6" t="s">
         <v>654</v>
       </c>
-      <c r="F102" s="9" t="s">
+      <c r="F103" s="9" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>520</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -4783,39 +4796,39 @@
         <v>230</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>290</v>
+        <v>229</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>290</v>
+        <v>229</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>291</v>
+        <v>231</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>751</v>
+        <v>230</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>645</v>
+        <v>290</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>644</v>
+        <v>290</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>643</v>
+        <v>291</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>521</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>641</v>
+        <v>292</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -4823,116 +4836,116 @@
         <v>751</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>4</v>
+        <v>645</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E106" s="6" t="s">
-        <v>647</v>
+        <v>642</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>643</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>6</v>
+        <v>641</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>571</v>
+        <v>751</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>678</v>
+        <v>4</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>681</v>
+        <v>646</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>679</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>682</v>
+        <v>5</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>647</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>571</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>471</v>
+        <v>678</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>476</v>
+        <v>681</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>472</v>
+        <v>679</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>682</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>571</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>19</v>
+        <v>471</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>20</v>
+        <v>476</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>21</v>
+        <v>493</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>472</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>571</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>529</v>
+        <v>19</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>574</v>
+        <v>20</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>560</v>
-      </c>
-      <c r="E110" s="6" t="s">
-        <v>530</v>
+        <v>21</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>571</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>478</v>
+        <v>529</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>492</v>
+        <v>574</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>494</v>
+        <v>560</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>491</v>
+        <v>530</v>
       </c>
       <c r="F111" s="9" t="s">
-        <v>479</v>
+        <v>499</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -4940,19 +4953,19 @@
         <v>571</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>742</v>
+        <v>478</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>747</v>
+        <v>492</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>740</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>739</v>
+        <v>494</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>491</v>
       </c>
       <c r="F112" s="9" t="s">
-        <v>741</v>
+        <v>479</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -4960,19 +4973,19 @@
         <v>571</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>621</v>
+        <v>742</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>625</v>
+        <v>747</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>623</v>
+        <v>740</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>622</v>
+        <v>739</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>624</v>
+        <v>741</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -4980,19 +4993,19 @@
         <v>571</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>511</v>
+        <v>621</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>549</v>
+        <v>625</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>547</v>
-      </c>
-      <c r="E114" s="6" t="s">
-        <v>512</v>
+        <v>623</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>622</v>
       </c>
       <c r="F114" s="9" t="s">
-        <v>548</v>
+        <v>624</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -5000,19 +5013,19 @@
         <v>571</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>396</v>
+        <v>511</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>397</v>
+        <v>549</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>398</v>
+        <v>547</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>399</v>
+        <v>548</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -5020,19 +5033,19 @@
         <v>571</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>589</v>
+        <v>396</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>594</v>
+        <v>397</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>592</v>
-      </c>
-      <c r="E116" s="5" t="s">
-        <v>590</v>
+        <v>398</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>507</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>593</v>
+        <v>399</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -5040,19 +5053,19 @@
         <v>571</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>501</v>
+        <v>589</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>502</v>
+        <v>594</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>559</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>503</v>
+        <v>592</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>590</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>558</v>
+        <v>593</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -5060,19 +5073,19 @@
         <v>571</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>588</v>
+        <v>501</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>586</v>
+        <v>502</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>584</v>
-      </c>
-      <c r="E118" s="5" t="s">
-        <v>591</v>
+        <v>559</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>503</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>585</v>
+        <v>558</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -5080,19 +5093,19 @@
         <v>571</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>575</v>
+        <v>588</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>576</v>
+        <v>586</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>577</v>
+        <v>591</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -5100,39 +5113,39 @@
         <v>571</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>337</v>
+        <v>575</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>338</v>
+        <v>576</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="E120" s="6" t="s">
-        <v>451</v>
+        <v>578</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>577</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>571</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>508</v>
+        <v>337</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>509</v>
+        <v>338</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>551</v>
+        <v>339</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>510</v>
+        <v>451</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>436</v>
+        <v>726</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -5140,79 +5153,79 @@
         <v>571</v>
       </c>
       <c r="B122" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="E122" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="F122" s="9" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A123" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="B123" s="5" t="s">
         <v>616</v>
       </c>
-      <c r="C122" s="5" t="s">
+      <c r="C123" s="5" t="s">
         <v>619</v>
       </c>
-      <c r="D122" s="5" t="s">
+      <c r="D123" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="E122" s="5" t="s">
+      <c r="E123" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="F122" s="9" t="s">
+      <c r="F123" s="9" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D123" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="F123" s="9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>233</v>
+        <v>178</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>234</v>
+        <v>179</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>235</v>
+        <v>180</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>81</v>
+        <v>233</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>82</v>
+        <v>234</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>84</v>
+        <v>235</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>451</v>
+        <v>522</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>85</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -5220,16 +5233,19 @@
         <v>83</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>545</v>
+        <v>451</v>
+      </c>
+      <c r="F126" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -5237,36 +5253,36 @@
         <v>83</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>293</v>
+        <v>102</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>293</v>
+        <v>102</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>294</v>
+        <v>103</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="F127" s="9" t="s">
-        <v>295</v>
+        <v>545</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
-        <v>193</v>
+        <v>83</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>715</v>
+        <v>293</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>715</v>
+        <v>293</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>716</v>
-      </c>
-      <c r="E128" s="5" t="s">
-        <v>451</v>
+        <v>294</v>
+      </c>
+      <c r="E128" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="F128" s="9" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -5274,59 +5290,56 @@
         <v>193</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>191</v>
+        <v>715</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>192</v>
+        <v>715</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="E129" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="E129" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="F129" s="9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>193</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>451</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>193</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>376</v>
+        <v>196</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>377</v>
+        <v>197</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>378</v>
+        <v>198</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>513</v>
+        <v>451</v>
       </c>
       <c r="F131" s="9" t="s">
-        <v>379</v>
+        <v>199</v>
       </c>
     </row>
     <row r="132" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5334,19 +5347,19 @@
         <v>193</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>218</v>
+        <v>376</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>219</v>
+        <v>377</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>220</v>
+        <v>378</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="F132" s="9" t="s">
-        <v>221</v>
+        <v>379</v>
       </c>
     </row>
     <row r="133" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5354,19 +5367,19 @@
         <v>193</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>518</v>
+        <v>218</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>304</v>
+        <v>219</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>569</v>
+        <v>220</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="F133" s="9" t="s">
-        <v>546</v>
+        <v>221</v>
       </c>
     </row>
     <row r="134" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5374,59 +5387,59 @@
         <v>193</v>
       </c>
       <c r="B134" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="F134" s="9" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B135" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="C134" s="5" t="s">
+      <c r="C135" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D134" s="5" t="s">
+      <c r="D135" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="E134" s="6" t="s">
+      <c r="E135" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="F134" s="9" t="s">
+      <c r="F135" s="9" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A135" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C135" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="D135" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="E135" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="F135" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>300</v>
+        <v>237</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>301</v>
+        <v>237</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>302</v>
+        <v>238</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F136" s="9" t="s">
-        <v>303</v>
+        <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5434,19 +5447,19 @@
         <v>118</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>117</v>
+        <v>300</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>117</v>
+        <v>301</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>119</v>
+        <v>302</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="F137" s="9" t="s">
-        <v>120</v>
+        <v>303</v>
       </c>
     </row>
     <row r="138" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5454,59 +5467,59 @@
         <v>118</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>326</v>
+        <v>117</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>327</v>
+        <v>117</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>328</v>
+        <v>119</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F138" s="9" t="s">
-        <v>329</v>
+        <v>120</v>
       </c>
     </row>
     <row r="139" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
-        <v>632</v>
+        <v>118</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>655</v>
+        <v>326</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>658</v>
+        <v>327</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>657</v>
+        <v>328</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>656</v>
+        <v>515</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>632</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>627</v>
+        <v>655</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>629</v>
+        <v>658</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>631</v>
-      </c>
-      <c r="E140" s="5" t="s">
-        <v>628</v>
+        <v>657</v>
+      </c>
+      <c r="E140" s="6" t="s">
+        <v>656</v>
       </c>
       <c r="F140" s="9" t="s">
-        <v>630</v>
+        <v>345</v>
       </c>
     </row>
     <row r="141" spans="1:6" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5514,39 +5527,39 @@
         <v>632</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>404</v>
+        <v>627</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>405</v>
+        <v>629</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="E141" s="6" t="s">
-        <v>665</v>
+        <v>631</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>628</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>632</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>651</v>
+        <v>404</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>650</v>
+        <v>405</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="E142" s="5" t="s">
-        <v>451</v>
+        <v>406</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>665</v>
       </c>
       <c r="F142" s="9" t="s">
-        <v>653</v>
+        <v>407</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
@@ -5554,19 +5567,19 @@
         <v>632</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>673</v>
+        <v>651</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>674</v>
+        <v>650</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>676</v>
+        <v>652</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>675</v>
+        <v>451</v>
       </c>
       <c r="F143" s="9" t="s">
-        <v>677</v>
+        <v>653</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -5574,39 +5587,39 @@
         <v>632</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>767</v>
+        <v>673</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>768</v>
+        <v>674</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>769</v>
+        <v>676</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>770</v>
+        <v>675</v>
       </c>
       <c r="F144" s="9" t="s">
-        <v>771</v>
+        <v>677</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
-        <v>58</v>
+        <v>632</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>57</v>
+        <v>767</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>669</v>
+        <v>768</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E145" s="6" t="s">
-        <v>667</v>
+        <v>769</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>770</v>
       </c>
       <c r="F145" s="9" t="s">
-        <v>60</v>
+        <v>771</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -5614,59 +5627,59 @@
         <v>58</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>383</v>
+        <v>57</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>384</v>
+        <v>669</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>603</v>
+        <v>59</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>602</v>
+        <v>667</v>
       </c>
       <c r="F146" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>90</v>
+        <v>383</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>671</v>
+        <v>384</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>670</v>
+        <v>603</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>672</v>
+        <v>602</v>
       </c>
       <c r="F147" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>138</v>
+        <v>671</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>139</v>
+        <v>670</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>542</v>
+        <v>672</v>
       </c>
       <c r="F148" s="9" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
@@ -5674,39 +5687,39 @@
         <v>58</v>
       </c>
       <c r="B149" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="F149" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B150" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C149" s="5" t="s">
+      <c r="C150" s="5" t="s">
         <v>648</v>
       </c>
-      <c r="D149" s="5" t="s">
+      <c r="D150" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E149" s="6" t="s">
+      <c r="E150" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="F149" s="9" t="s">
+      <c r="F150" s="9" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A150" s="5" t="s">
-        <v>755</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="C150" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D150" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E150" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="F150" s="9" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -5714,19 +5727,19 @@
         <v>755</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>309</v>
+        <v>244</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>310</v>
+        <v>244</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>245</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>604</v>
+        <v>525</v>
       </c>
       <c r="F151" s="9" t="s">
-        <v>311</v>
+        <v>246</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -5734,79 +5747,79 @@
         <v>755</v>
       </c>
       <c r="B152" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E152" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A153" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="B153" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C152" s="5" t="s">
+      <c r="C153" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="D152" s="5" t="s">
+      <c r="D153" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E152" s="6" t="s">
+      <c r="E153" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="F152" s="9" t="s">
+      <c r="F153" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A153" s="5" t="s">
+    <row r="154" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A154" s="5" t="s">
         <v>756</v>
       </c>
-      <c r="B153" s="5" t="s">
+      <c r="B154" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C153" s="5" t="s">
+      <c r="C154" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D153" s="5" t="s">
+      <c r="D154" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E153" s="6" t="s">
+      <c r="E154" s="6" t="s">
         <v>451</v>
       </c>
-      <c r="F153" s="9" t="s">
+      <c r="F154" s="9" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" s="6" t="s">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="B154" s="6" t="s">
+      <c r="B155" s="6" t="s">
         <v>565</v>
       </c>
-      <c r="C154" s="6" t="s">
+      <c r="C155" s="6" t="s">
         <v>565</v>
       </c>
-      <c r="D154" s="6" t="s">
+      <c r="D155" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="E154" s="6" t="s">
+      <c r="E155" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="F154" s="9" t="s">
+      <c r="F155" s="9" t="s">
         <v>566</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A155" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="B155" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C155" s="5" t="s">
-        <v>610</v>
-      </c>
-      <c r="D155" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="E155" s="6" t="s">
-        <v>609</v>
-      </c>
-      <c r="F155" s="9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -5814,19 +5827,19 @@
         <v>756</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>269</v>
+        <v>79</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>269</v>
+        <v>610</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>270</v>
+        <v>757</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>451</v>
+        <v>609</v>
       </c>
       <c r="F156" s="9" t="s">
-        <v>271</v>
+        <v>80</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -5834,19 +5847,19 @@
         <v>756</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>400</v>
+        <v>269</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>401</v>
+        <v>269</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>402</v>
+        <v>270</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>649</v>
+        <v>451</v>
       </c>
       <c r="F157" s="9" t="s">
-        <v>403</v>
+        <v>271</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
@@ -5854,99 +5867,99 @@
         <v>756</v>
       </c>
       <c r="B158" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="D158" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="B159" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C158" s="5" t="s">
+      <c r="C159" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D158" s="5" t="s">
+      <c r="D159" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E158" s="6" t="s">
+      <c r="E159" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="F158" s="9" t="s">
+      <c r="F159" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A159" s="5" t="s">
-        <v>758</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C159" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="D159" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E159" s="6" t="s">
-        <v>664</v>
-      </c>
-      <c r="F159" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
         <v>758</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>659</v>
+        <v>92</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>661</v>
-      </c>
-      <c r="E160" s="5" t="s">
-        <v>660</v>
+        <v>93</v>
+      </c>
+      <c r="E160" s="6" t="s">
+        <v>664</v>
       </c>
       <c r="F160" s="9" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
         <v>758</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>763</v>
+        <v>659</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>764</v>
+        <v>659</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>765</v>
+        <v>661</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>451</v>
+        <v>660</v>
       </c>
       <c r="F161" s="9" t="s">
-        <v>766</v>
+        <v>662</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A162" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>15</v>
+        <v>763</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>16</v>
+        <v>764</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E162" s="6" t="s">
-        <v>528</v>
+        <v>765</v>
+      </c>
+      <c r="E162" s="5" t="s">
+        <v>451</v>
       </c>
       <c r="F162" s="9" t="s">
-        <v>18</v>
+        <v>766</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -5954,118 +5967,138 @@
         <v>759</v>
       </c>
       <c r="B163" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D163" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E163" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="F163" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A164" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="B164" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="C163" s="5" t="s">
+      <c r="C164" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="D163" s="5" t="s">
+      <c r="D164" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="E163" s="6" t="s">
+      <c r="E164" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="F163" s="9" t="s">
+      <c r="F164" s="9" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A164" s="5" t="s">
+    <row r="165" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A165" s="5" t="s">
         <v>760</v>
       </c>
-      <c r="B164" s="5" t="s">
+      <c r="B165" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C164" s="5" t="s">
+      <c r="C165" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D164" s="5" t="s">
+      <c r="D165" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E164" s="6" t="s">
+      <c r="E165" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="F164" s="9" t="s">
+      <c r="F165" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A165" s="5" t="s">
-        <v>761</v>
-      </c>
-      <c r="B165" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C165" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D165" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E165" s="6" t="s">
-        <v>684</v>
-      </c>
-      <c r="F165" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>761</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>666</v>
+        <v>684</v>
       </c>
       <c r="F166" s="9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>761</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>254</v>
+        <v>174</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>255</v>
+        <v>175</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>256</v>
+        <v>176</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>451</v>
+        <v>666</v>
       </c>
       <c r="F167" s="9" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>761</v>
       </c>
       <c r="B168" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E168" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="F168" s="9" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A169" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="B169" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="C168" s="5" t="s">
+      <c r="C169" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="D168" s="5" t="s">
+      <c r="D169" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="E168" s="6" t="s">
+      <c r="E169" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="F168" s="9" t="s">
+      <c r="F169" s="9" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6139,106 +6172,108 @@
     <hyperlink ref="F67" r:id="rId62"/>
     <hyperlink ref="F68" r:id="rId63"/>
     <hyperlink ref="F69" r:id="rId64"/>
-    <hyperlink ref="F70" r:id="rId65"/>
-    <hyperlink ref="F71" r:id="rId66"/>
-    <hyperlink ref="F72" r:id="rId67"/>
-    <hyperlink ref="F73" r:id="rId68"/>
-    <hyperlink ref="F74" r:id="rId69"/>
-    <hyperlink ref="F75" r:id="rId70"/>
-    <hyperlink ref="F77" r:id="rId71"/>
-    <hyperlink ref="F78" r:id="rId72"/>
-    <hyperlink ref="F80" r:id="rId73"/>
-    <hyperlink ref="F81" r:id="rId74"/>
-    <hyperlink ref="F82" r:id="rId75"/>
-    <hyperlink ref="F83" r:id="rId76"/>
-    <hyperlink ref="F84" r:id="rId77"/>
-    <hyperlink ref="F85" r:id="rId78"/>
-    <hyperlink ref="F86" r:id="rId79"/>
-    <hyperlink ref="F87" r:id="rId80"/>
-    <hyperlink ref="F88" r:id="rId81"/>
-    <hyperlink ref="F89" r:id="rId82"/>
-    <hyperlink ref="F90" r:id="rId83"/>
-    <hyperlink ref="F91" r:id="rId84"/>
-    <hyperlink ref="F92" r:id="rId85"/>
-    <hyperlink ref="F93" r:id="rId86"/>
-    <hyperlink ref="F94" r:id="rId87"/>
-    <hyperlink ref="F95" r:id="rId88"/>
-    <hyperlink ref="F96" r:id="rId89"/>
-    <hyperlink ref="F97" r:id="rId90"/>
-    <hyperlink ref="F98" r:id="rId91" location="debugger"/>
-    <hyperlink ref="F99" r:id="rId92"/>
-    <hyperlink ref="F100" r:id="rId93"/>
-    <hyperlink ref="F101" r:id="rId94"/>
-    <hyperlink ref="F102" r:id="rId95"/>
-    <hyperlink ref="F103" r:id="rId96"/>
-    <hyperlink ref="F104" r:id="rId97"/>
-    <hyperlink ref="F105" r:id="rId98"/>
-    <hyperlink ref="F106" r:id="rId99"/>
-    <hyperlink ref="F107" r:id="rId100"/>
-    <hyperlink ref="F108" r:id="rId101"/>
-    <hyperlink ref="F109" r:id="rId102"/>
-    <hyperlink ref="F110" r:id="rId103"/>
-    <hyperlink ref="F111" r:id="rId104"/>
-    <hyperlink ref="F112" r:id="rId105"/>
-    <hyperlink ref="F113" r:id="rId106"/>
-    <hyperlink ref="F114" r:id="rId107"/>
-    <hyperlink ref="F115" r:id="rId108"/>
-    <hyperlink ref="F116" r:id="rId109"/>
-    <hyperlink ref="F117" r:id="rId110"/>
-    <hyperlink ref="F118" r:id="rId111"/>
-    <hyperlink ref="F119" r:id="rId112"/>
-    <hyperlink ref="F120" r:id="rId113"/>
-    <hyperlink ref="F121" r:id="rId114"/>
-    <hyperlink ref="F122" r:id="rId115"/>
-    <hyperlink ref="F123" r:id="rId116"/>
-    <hyperlink ref="F124" r:id="rId117"/>
-    <hyperlink ref="F125" r:id="rId118"/>
-    <hyperlink ref="F127" r:id="rId119"/>
-    <hyperlink ref="F129" r:id="rId120"/>
-    <hyperlink ref="F130" r:id="rId121"/>
-    <hyperlink ref="F131" r:id="rId122"/>
-    <hyperlink ref="F132" r:id="rId123"/>
-    <hyperlink ref="F133" r:id="rId124"/>
-    <hyperlink ref="F134" r:id="rId125"/>
-    <hyperlink ref="F135" r:id="rId126"/>
-    <hyperlink ref="F136" r:id="rId127"/>
-    <hyperlink ref="F137" r:id="rId128"/>
-    <hyperlink ref="F138" r:id="rId129"/>
-    <hyperlink ref="F139" r:id="rId130"/>
-    <hyperlink ref="F140" r:id="rId131"/>
-    <hyperlink ref="F141" r:id="rId132"/>
-    <hyperlink ref="F142" r:id="rId133"/>
-    <hyperlink ref="F143" r:id="rId134"/>
-    <hyperlink ref="F145" r:id="rId135"/>
-    <hyperlink ref="F146" r:id="rId136"/>
-    <hyperlink ref="F147" r:id="rId137"/>
-    <hyperlink ref="F148" r:id="rId138"/>
-    <hyperlink ref="F149" r:id="rId139"/>
-    <hyperlink ref="F150" r:id="rId140"/>
-    <hyperlink ref="F151" r:id="rId141"/>
-    <hyperlink ref="F152" r:id="rId142"/>
-    <hyperlink ref="F153" r:id="rId143"/>
-    <hyperlink ref="F154" r:id="rId144"/>
-    <hyperlink ref="F155" r:id="rId145"/>
-    <hyperlink ref="F156" r:id="rId146"/>
-    <hyperlink ref="F157" r:id="rId147"/>
-    <hyperlink ref="F158" r:id="rId148"/>
-    <hyperlink ref="F159" r:id="rId149"/>
-    <hyperlink ref="F160" r:id="rId150"/>
-    <hyperlink ref="F162" r:id="rId151"/>
-    <hyperlink ref="F163" r:id="rId152"/>
-    <hyperlink ref="F164" r:id="rId153"/>
-    <hyperlink ref="F165" r:id="rId154"/>
-    <hyperlink ref="F166" r:id="rId155"/>
-    <hyperlink ref="F167" r:id="rId156"/>
-    <hyperlink ref="F168" r:id="rId157"/>
-    <hyperlink ref="F161" r:id="rId158"/>
-    <hyperlink ref="F144" r:id="rId159"/>
+    <hyperlink ref="F71" r:id="rId65"/>
+    <hyperlink ref="F72" r:id="rId66"/>
+    <hyperlink ref="F73" r:id="rId67"/>
+    <hyperlink ref="F74" r:id="rId68"/>
+    <hyperlink ref="F75" r:id="rId69"/>
+    <hyperlink ref="F76" r:id="rId70"/>
+    <hyperlink ref="F78" r:id="rId71"/>
+    <hyperlink ref="F79" r:id="rId72"/>
+    <hyperlink ref="F81" r:id="rId73"/>
+    <hyperlink ref="F82" r:id="rId74"/>
+    <hyperlink ref="F83" r:id="rId75"/>
+    <hyperlink ref="F84" r:id="rId76"/>
+    <hyperlink ref="F85" r:id="rId77"/>
+    <hyperlink ref="F86" r:id="rId78"/>
+    <hyperlink ref="F87" r:id="rId79"/>
+    <hyperlink ref="F88" r:id="rId80"/>
+    <hyperlink ref="F89" r:id="rId81"/>
+    <hyperlink ref="F90" r:id="rId82"/>
+    <hyperlink ref="F91" r:id="rId83"/>
+    <hyperlink ref="F92" r:id="rId84"/>
+    <hyperlink ref="F93" r:id="rId85"/>
+    <hyperlink ref="F94" r:id="rId86"/>
+    <hyperlink ref="F95" r:id="rId87"/>
+    <hyperlink ref="F96" r:id="rId88"/>
+    <hyperlink ref="F97" r:id="rId89"/>
+    <hyperlink ref="F98" r:id="rId90"/>
+    <hyperlink ref="F99" r:id="rId91" location="debugger"/>
+    <hyperlink ref="F100" r:id="rId92"/>
+    <hyperlink ref="F101" r:id="rId93"/>
+    <hyperlink ref="F102" r:id="rId94"/>
+    <hyperlink ref="F103" r:id="rId95"/>
+    <hyperlink ref="F104" r:id="rId96"/>
+    <hyperlink ref="F105" r:id="rId97"/>
+    <hyperlink ref="F106" r:id="rId98"/>
+    <hyperlink ref="F107" r:id="rId99"/>
+    <hyperlink ref="F108" r:id="rId100"/>
+    <hyperlink ref="F109" r:id="rId101"/>
+    <hyperlink ref="F110" r:id="rId102"/>
+    <hyperlink ref="F111" r:id="rId103"/>
+    <hyperlink ref="F112" r:id="rId104"/>
+    <hyperlink ref="F113" r:id="rId105"/>
+    <hyperlink ref="F114" r:id="rId106"/>
+    <hyperlink ref="F115" r:id="rId107"/>
+    <hyperlink ref="F116" r:id="rId108"/>
+    <hyperlink ref="F117" r:id="rId109"/>
+    <hyperlink ref="F118" r:id="rId110"/>
+    <hyperlink ref="F119" r:id="rId111"/>
+    <hyperlink ref="F120" r:id="rId112"/>
+    <hyperlink ref="F121" r:id="rId113"/>
+    <hyperlink ref="F122" r:id="rId114"/>
+    <hyperlink ref="F123" r:id="rId115"/>
+    <hyperlink ref="F124" r:id="rId116"/>
+    <hyperlink ref="F125" r:id="rId117"/>
+    <hyperlink ref="F126" r:id="rId118"/>
+    <hyperlink ref="F128" r:id="rId119"/>
+    <hyperlink ref="F130" r:id="rId120"/>
+    <hyperlink ref="F131" r:id="rId121"/>
+    <hyperlink ref="F132" r:id="rId122"/>
+    <hyperlink ref="F133" r:id="rId123"/>
+    <hyperlink ref="F134" r:id="rId124"/>
+    <hyperlink ref="F135" r:id="rId125"/>
+    <hyperlink ref="F136" r:id="rId126"/>
+    <hyperlink ref="F137" r:id="rId127"/>
+    <hyperlink ref="F138" r:id="rId128"/>
+    <hyperlink ref="F139" r:id="rId129"/>
+    <hyperlink ref="F140" r:id="rId130"/>
+    <hyperlink ref="F141" r:id="rId131"/>
+    <hyperlink ref="F142" r:id="rId132"/>
+    <hyperlink ref="F143" r:id="rId133"/>
+    <hyperlink ref="F144" r:id="rId134"/>
+    <hyperlink ref="F146" r:id="rId135"/>
+    <hyperlink ref="F147" r:id="rId136"/>
+    <hyperlink ref="F148" r:id="rId137"/>
+    <hyperlink ref="F149" r:id="rId138"/>
+    <hyperlink ref="F150" r:id="rId139"/>
+    <hyperlink ref="F151" r:id="rId140"/>
+    <hyperlink ref="F152" r:id="rId141"/>
+    <hyperlink ref="F153" r:id="rId142"/>
+    <hyperlink ref="F154" r:id="rId143"/>
+    <hyperlink ref="F155" r:id="rId144"/>
+    <hyperlink ref="F156" r:id="rId145"/>
+    <hyperlink ref="F157" r:id="rId146"/>
+    <hyperlink ref="F158" r:id="rId147"/>
+    <hyperlink ref="F159" r:id="rId148"/>
+    <hyperlink ref="F160" r:id="rId149"/>
+    <hyperlink ref="F161" r:id="rId150"/>
+    <hyperlink ref="F163" r:id="rId151"/>
+    <hyperlink ref="F164" r:id="rId152"/>
+    <hyperlink ref="F165" r:id="rId153"/>
+    <hyperlink ref="F166" r:id="rId154"/>
+    <hyperlink ref="F167" r:id="rId155"/>
+    <hyperlink ref="F168" r:id="rId156"/>
+    <hyperlink ref="F169" r:id="rId157"/>
+    <hyperlink ref="F162" r:id="rId158"/>
+    <hyperlink ref="F145" r:id="rId159"/>
+    <hyperlink ref="F70" r:id="rId160"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId160"/>
-  <webPublishItems count="1">
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId161"/>
+  <webPublishItems count="2">
     <webPublishItem id="28559" divId="remnux-tools_28559" sourceType="sheet" destinationFile="C:\Users\Lenny\Documents\SANS Institute\REMnux\v6\remnux-tools-sheet.html" title="REMnux Tools"/>
+    <webPublishItem id="24838" divId="remnux-tools-sheet_24838" sourceType="sheet" destinationFile="C:\Users\Lenny\Documents\SANS Institute\REMnux\v6\remnux-tools-sheet.htm"/>
   </webPublishItems>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated remnux-tools-sheet to reflect Thug now being a Docker container.
</commit_message>
<xml_diff>
--- a/remnux-tools-sheet.xlsx
+++ b/remnux-tools-sheet.xlsx
@@ -1734,9 +1734,6 @@
     <t>thug.py</t>
   </si>
   <si>
-    <t>remnux-thug (APT)</t>
-  </si>
-  <si>
     <t>remnux-trid (APT)</t>
   </si>
   <si>
@@ -2491,6 +2488,9 @@
   </si>
   <si>
     <t>cd /opt/remnux-viper &amp;&amp; ./viper.py</t>
+  </si>
+  <si>
+    <t>remnux/thug (Docker)</t>
   </si>
 </sst>
 </file>
@@ -2863,7 +2863,7 @@
   <dimension ref="A1:F179"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -2972,7 +2972,7 @@
         <v>197</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>198</v>
@@ -3000,27 +3000,27 @@
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>706</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="F7" s="9" t="s">
         <v>708</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>707</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>278</v>
@@ -3063,19 +3063,19 @@
         <v>183</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>703</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>702</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>704</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -3092,7 +3092,7 @@
         <v>273</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>274</v>
@@ -3143,19 +3143,19 @@
         <v>51</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>728</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>729</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>372</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>730</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3172,10 +3172,10 @@
         <v>219</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -3212,7 +3212,7 @@
         <v>372</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>373</v>
@@ -3226,7 +3226,7 @@
         <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>33</v>
@@ -3266,13 +3266,13 @@
         <v>54</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>56</v>
@@ -3283,10 +3283,10 @@
         <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>168</v>
@@ -3323,13 +3323,13 @@
         <v>282</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>283</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>284</v>
@@ -3343,13 +3343,13 @@
         <v>311</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>691</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>693</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>692</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>312</v>
@@ -3363,13 +3363,13 @@
         <v>7</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>10</v>
@@ -3389,7 +3389,7 @@
         <v>345</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>346</v>
@@ -3400,19 +3400,19 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>379</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -3420,19 +3420,19 @@
         <v>8</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>761</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>762</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>763</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>438</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -3509,7 +3509,7 @@
         <v>379</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>380</v>
@@ -3520,19 +3520,19 @@
         <v>8</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>263</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3552,7 +3552,7 @@
         <v>477</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -3560,19 +3560,19 @@
         <v>8</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>379</v>
       </c>
       <c r="E35" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>695</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -3609,7 +3609,7 @@
         <v>122</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>568</v>
+        <v>818</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>123</v>
@@ -3660,19 +3660,19 @@
         <v>70</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>721</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>722</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>439</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -3680,19 +3680,19 @@
         <v>70</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>776</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>777</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>778</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="F41" s="9" t="s">
         <v>779</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -3700,19 +3700,19 @@
         <v>70</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="F42" s="9" t="s">
         <v>679</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>674</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>678</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -3740,10 +3740,10 @@
         <v>70</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>716</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>717</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>381</v>
@@ -3752,7 +3752,7 @@
         <v>439</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -3760,19 +3760,19 @@
         <v>70</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>673</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>676</v>
-      </c>
-      <c r="D45" s="5" t="s">
+      <c r="E45" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="F45" s="9" t="s">
         <v>674</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>681</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -3780,10 +3780,10 @@
         <v>70</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>381</v>
@@ -3792,7 +3792,7 @@
         <v>438</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -3832,7 +3832,7 @@
         <v>475</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3843,7 +3843,7 @@
         <v>252</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>253</v>
@@ -3949,10 +3949,10 @@
         <v>386</v>
       </c>
       <c r="E54" s="6" t="s">
+        <v>586</v>
+      </c>
+      <c r="F54" s="9" t="s">
         <v>587</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -3980,19 +3980,19 @@
         <v>1</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>797</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>797</v>
-      </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="6" t="s">
         <v>798</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="F56" s="9" t="s">
         <v>799</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -4000,19 +4000,19 @@
         <v>1</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>801</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>801</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="6" t="s">
         <v>802</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="F57" s="9" t="s">
         <v>803</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -4072,7 +4072,7 @@
         <v>438</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -4117,7 +4117,7 @@
         <v>161</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>162</v>
@@ -4137,7 +4137,7 @@
         <v>45</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>47</v>
@@ -4154,19 +4154,19 @@
         <v>46</v>
       </c>
       <c r="B65" s="5" t="s">
+        <v>581</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="D65" s="5" t="s">
+        <v>585</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>583</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>586</v>
-      </c>
-      <c r="E65" s="5" t="s">
+      <c r="F65" s="9" t="s">
         <v>584</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -4174,19 +4174,19 @@
         <v>46</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>785</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="D66" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>787</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="F66" s="9" t="s">
         <v>788</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -4314,19 +4314,19 @@
         <v>42</v>
       </c>
       <c r="B73" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>756</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="D73" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>757</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>760</v>
-      </c>
-      <c r="E73" s="6" t="s">
+      <c r="F73" s="9" t="s">
         <v>758</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -4397,13 +4397,13 @@
         <v>405</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>406</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>407</v>
@@ -4531,7 +4531,7 @@
         <v>412</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>413</v>
@@ -4551,7 +4551,7 @@
         <v>522</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>539</v>
@@ -4568,10 +4568,10 @@
         <v>128</v>
       </c>
       <c r="B86" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="C86" s="5" t="s">
         <v>811</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>812</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>539</v>
@@ -4580,7 +4580,7 @@
         <v>438</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -4591,7 +4591,7 @@
         <v>341</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>342</v>
@@ -4600,7 +4600,7 @@
         <v>447</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
@@ -4708,19 +4708,19 @@
         <v>12</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>438</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -4877,7 +4877,7 @@
         <v>425</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F101" s="9" t="s">
         <v>394</v>
@@ -4888,19 +4888,19 @@
         <v>109</v>
       </c>
       <c r="B102" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="D102" s="5" t="s">
         <v>793</v>
       </c>
-      <c r="C102" s="5" t="s">
-        <v>793</v>
-      </c>
-      <c r="D102" s="5" t="s">
+      <c r="E102" s="6" t="s">
         <v>794</v>
       </c>
-      <c r="E102" s="6" t="s">
+      <c r="F102" s="9" t="s">
         <v>795</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -4908,19 +4908,19 @@
         <v>109</v>
       </c>
       <c r="B103" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>790</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>790</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>791</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>439</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -4931,7 +4931,7 @@
         <v>108</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>110</v>
@@ -4948,7 +4948,7 @@
         <v>24</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>23</v>
@@ -4957,7 +4957,7 @@
         <v>25</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F105" s="9" t="s">
         <v>26</v>
@@ -4985,42 +4985,42 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B107" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="C107" s="5" t="s">
         <v>598</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="D107" s="5" t="s">
         <v>599</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>600</v>
       </c>
       <c r="E107" s="5" t="s">
         <v>438</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B108" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="C108" s="5" t="s">
         <v>815</v>
       </c>
-      <c r="C108" s="5" t="s">
-        <v>816</v>
-      </c>
       <c r="D108" s="5" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E108" s="5" t="s">
         <v>438</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -5057,7 +5057,7 @@
         <v>131</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F110" s="9" t="s">
         <v>132</v>
@@ -5105,39 +5105,39 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D113" s="5" t="s">
+        <v>628</v>
+      </c>
+      <c r="E113" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="E113" s="5" t="s">
-        <v>630</v>
-      </c>
       <c r="F113" s="9" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F114" s="9" t="s">
         <v>6</v>
@@ -5148,19 +5148,19 @@
         <v>558</v>
       </c>
       <c r="B115" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="D115" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="C115" s="5" t="s">
+      <c r="E115" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="F115" s="9" t="s">
         <v>666</v>
-      </c>
-      <c r="E115" s="5" t="s">
-        <v>669</v>
-      </c>
-      <c r="F115" s="9" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -5245,19 +5245,19 @@
         <v>558</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D120" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="F120" s="9" t="s">
         <v>725</v>
-      </c>
-      <c r="E120" s="5" t="s">
-        <v>724</v>
-      </c>
-      <c r="F120" s="9" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
@@ -5265,19 +5265,19 @@
         <v>558</v>
       </c>
       <c r="B121" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="E121" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="C121" s="5" t="s">
-        <v>612</v>
-      </c>
-      <c r="D121" s="5" t="s">
+      <c r="F121" s="9" t="s">
         <v>610</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>609</v>
-      </c>
-      <c r="F121" s="9" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
@@ -5325,19 +5325,19 @@
         <v>558</v>
       </c>
       <c r="B124" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="E124" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="C124" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="D124" s="5" t="s">
+      <c r="F124" s="9" t="s">
         <v>579</v>
-      </c>
-      <c r="E124" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="F124" s="9" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
@@ -5365,19 +5365,19 @@
         <v>558</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D126" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="F126" s="9" t="s">
         <v>571</v>
-      </c>
-      <c r="E126" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="F126" s="9" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
@@ -5417,7 +5417,7 @@
         <v>438</v>
       </c>
       <c r="F128" s="9" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
@@ -5445,19 +5445,19 @@
         <v>558</v>
       </c>
       <c r="B130" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="E130" s="5" t="s">
         <v>603</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="F130" s="9" t="s">
         <v>606</v>
-      </c>
-      <c r="D130" s="5" t="s">
-        <v>605</v>
-      </c>
-      <c r="E130" s="5" t="s">
-        <v>604</v>
-      </c>
-      <c r="F130" s="9" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
@@ -5562,19 +5562,19 @@
         <v>83</v>
       </c>
       <c r="B136" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="C136" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="C136" s="5" t="s">
+      <c r="D136" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="D136" s="5" t="s">
+      <c r="E136" s="6" t="s">
         <v>807</v>
       </c>
-      <c r="E136" s="6" t="s">
+      <c r="F136" s="9" t="s">
         <v>808</v>
-      </c>
-      <c r="F136" s="9" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
@@ -5582,13 +5582,13 @@
         <v>188</v>
       </c>
       <c r="B137" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="D137" s="5" t="s">
         <v>700</v>
-      </c>
-      <c r="C137" s="5" t="s">
-        <v>700</v>
-      </c>
-      <c r="D137" s="5" t="s">
-        <v>701</v>
       </c>
       <c r="E137" s="5" t="s">
         <v>438</v>
@@ -5796,19 +5796,19 @@
     </row>
     <row r="148" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B148" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="E148" s="6" t="s">
         <v>642</v>
-      </c>
-      <c r="C148" s="5" t="s">
-        <v>645</v>
-      </c>
-      <c r="D148" s="5" t="s">
-        <v>644</v>
-      </c>
-      <c r="E148" s="6" t="s">
-        <v>643</v>
       </c>
       <c r="F148" s="9" t="s">
         <v>340</v>
@@ -5816,27 +5816,27 @@
     </row>
     <row r="149" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B149" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="E149" s="5" t="s">
         <v>614</v>
       </c>
-      <c r="C149" s="5" t="s">
+      <c r="F149" s="9" t="s">
         <v>616</v>
-      </c>
-      <c r="D149" s="5" t="s">
-        <v>618</v>
-      </c>
-      <c r="E149" s="5" t="s">
-        <v>615</v>
-      </c>
-      <c r="F149" s="9" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="150" spans="1:6" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>395</v>
@@ -5848,7 +5848,7 @@
         <v>397</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F150" s="9" t="s">
         <v>398</v>
@@ -5856,62 +5856,62 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B151" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="D151" s="5" t="s">
         <v>638</v>
-      </c>
-      <c r="C151" s="5" t="s">
-        <v>637</v>
-      </c>
-      <c r="D151" s="5" t="s">
-        <v>639</v>
       </c>
       <c r="E151" s="5" t="s">
         <v>438</v>
       </c>
       <c r="F151" s="9" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B152" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="C152" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="C152" s="5" t="s">
+      <c r="D152" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="E152" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D152" s="5" t="s">
+      <c r="F152" s="9" t="s">
         <v>663</v>
-      </c>
-      <c r="E152" s="5" t="s">
-        <v>662</v>
-      </c>
-      <c r="F152" s="9" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B153" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="C153" s="5" t="s">
         <v>751</v>
       </c>
-      <c r="C153" s="5" t="s">
+      <c r="D153" s="5" t="s">
         <v>752</v>
       </c>
-      <c r="D153" s="5" t="s">
+      <c r="E153" s="5" t="s">
         <v>753</v>
       </c>
-      <c r="E153" s="5" t="s">
+      <c r="F153" s="9" t="s">
         <v>754</v>
-      </c>
-      <c r="F153" s="9" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
@@ -5922,13 +5922,13 @@
         <v>57</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E154" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F154" s="9" t="s">
         <v>60</v>
@@ -5945,10 +5945,10 @@
         <v>375</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F155" s="9" t="s">
         <v>376</v>
@@ -5962,13 +5962,13 @@
         <v>90</v>
       </c>
       <c r="C156" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="D156" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="E156" s="6" t="s">
         <v>658</v>
-      </c>
-      <c r="D156" s="5" t="s">
-        <v>657</v>
-      </c>
-      <c r="E156" s="6" t="s">
-        <v>659</v>
       </c>
       <c r="F156" s="9" t="s">
         <v>91</v>
@@ -5982,7 +5982,7 @@
         <v>137</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>138</v>
@@ -6002,7 +6002,7 @@
         <v>143</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>144</v>
@@ -6016,7 +6016,7 @@
     </row>
     <row r="159" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>239</v>
@@ -6036,27 +6036,27 @@
     </row>
     <row r="160" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E160" s="6" t="s">
         <v>438</v>
       </c>
       <c r="F160" s="9" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B161" s="5" t="s">
         <v>304</v>
@@ -6068,7 +6068,7 @@
         <v>240</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F161" s="9" t="s">
         <v>306</v>
@@ -6076,19 +6076,19 @@
     </row>
     <row r="162" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>140</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>141</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F162" s="9" t="s">
         <v>142</v>
@@ -6096,7 +6096,7 @@
     </row>
     <row r="163" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B163" s="5" t="s">
         <v>177</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="6" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B164" s="6" t="s">
         <v>552</v>
@@ -6136,19 +6136,19 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B165" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F165" s="9" t="s">
         <v>80</v>
@@ -6156,7 +6156,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>264</v>
@@ -6176,7 +6176,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>391</v>
@@ -6188,7 +6188,7 @@
         <v>393</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F167" s="9" t="s">
         <v>394</v>
@@ -6196,7 +6196,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B168" s="5" t="s">
         <v>104</v>
@@ -6216,19 +6216,19 @@
     </row>
     <row r="169" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B169" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F169" s="9" t="s">
         <v>94</v>
@@ -6236,67 +6236,67 @@
     </row>
     <row r="170" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B170" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="C170" s="5" t="s">
         <v>765</v>
       </c>
-      <c r="C170" s="5" t="s">
+      <c r="D170" s="5" t="s">
         <v>766</v>
       </c>
-      <c r="D170" s="5" t="s">
+      <c r="E170" s="6" t="s">
         <v>767</v>
       </c>
-      <c r="E170" s="6" t="s">
+      <c r="F170" s="9" t="s">
         <v>768</v>
-      </c>
-      <c r="F170" s="9" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B171" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="E171" s="5" t="s">
         <v>646</v>
       </c>
-      <c r="C171" s="5" t="s">
-        <v>646</v>
-      </c>
-      <c r="D171" s="5" t="s">
+      <c r="F171" s="9" t="s">
         <v>648</v>
-      </c>
-      <c r="E171" s="5" t="s">
-        <v>647</v>
-      </c>
-      <c r="F171" s="9" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B172" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="C172" s="5" t="s">
         <v>747</v>
       </c>
-      <c r="C172" s="5" t="s">
+      <c r="D172" s="5" t="s">
         <v>748</v>
-      </c>
-      <c r="D172" s="5" t="s">
-        <v>749</v>
       </c>
       <c r="E172" s="5" t="s">
         <v>438</v>
       </c>
       <c r="F172" s="9" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B173" s="5" t="s">
         <v>15</v>
@@ -6316,7 +6316,7 @@
     </row>
     <row r="174" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A174" s="5" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B174" s="5" t="s">
         <v>267</v>
@@ -6336,7 +6336,7 @@
     </row>
     <row r="175" spans="1:6" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B175" s="5" t="s">
         <v>86</v>
@@ -6356,7 +6356,7 @@
     </row>
     <row r="176" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B176" s="5" t="s">
         <v>164</v>
@@ -6368,7 +6368,7 @@
         <v>166</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F176" s="9" t="s">
         <v>167</v>
@@ -6376,7 +6376,7 @@
     </row>
     <row r="177" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A177" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B177" s="5" t="s">
         <v>169</v>
@@ -6388,7 +6388,7 @@
         <v>171</v>
       </c>
       <c r="E177" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F177" s="9" t="s">
         <v>172</v>
@@ -6396,7 +6396,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B178" s="5" t="s">
         <v>249</v>
@@ -6411,12 +6411,12 @@
         <v>438</v>
       </c>
       <c r="F178" s="9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B179" s="5" t="s">
         <v>307</v>

</xml_diff>